<commit_message>
Schematic Updates & Parts List Updates
</commit_message>
<xml_diff>
--- a/Documents/partsList.xlsx
+++ b/Documents/partsList.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DESIGN 1\Github\Senior_Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\GitHub\Senior_Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9555"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DSP Board" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>4xTL07</t>
   </si>
@@ -87,13 +87,82 @@
   </si>
   <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>Item Number</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>176-Pin QFP</t>
+  </si>
+  <si>
+    <t>TMS320F28335</t>
+  </si>
+  <si>
+    <t>Digital Signal Processor</t>
+  </si>
+  <si>
+    <t>ADS8320</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>Audio Sampler</t>
+  </si>
+  <si>
+    <t>TPS70351</t>
+  </si>
+  <si>
+    <t>24-Pin PowerPAD TSSOP</t>
+  </si>
+  <si>
+    <t>5.0V to 3.3V/1.8V Power Delivery and Sequencing</t>
+  </si>
+  <si>
+    <t>Epson Oscillator</t>
+  </si>
+  <si>
+    <t>4-Pin (Unique)</t>
+  </si>
+  <si>
+    <t>Oscillator Source for DSP Clock</t>
+  </si>
+  <si>
+    <t>Audio BandPass Filter Op-Amps</t>
+  </si>
+  <si>
+    <t>Audio PreAmp Op-Amps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +178,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,15 +208,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -448,16 +540,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,32 +566,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -498,26 +599,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -525,17 +627,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -543,19 +645,331 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>13</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>19</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{DFD1F882-806F-4D89-8EB5-61B8A146F8DF}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>